<commit_message>
updated with binary times
</commit_message>
<xml_diff>
--- a/index_serialization_times.xlsx
+++ b/index_serialization_times.xlsx
@@ -20,9 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
-  <si>
-    <t xml:space="preserve">Load Time from Disk Serialization – Average of 5 runs (secs)</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="13">
+  <si>
+    <t xml:space="preserve">Load Time from Disk Serialization – Text  data (secs)</t>
   </si>
   <si>
     <t xml:space="preserve">Mesh</t>
@@ -52,7 +52,13 @@
     <t xml:space="preserve">Optimal</t>
   </si>
   <si>
-    <t xml:space="preserve">Size of Serialized Data File (GB)</t>
+    <t xml:space="preserve">Size of Serialized Data File – Text data (GB)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Load Time from Disk Serialization – Binary data (secs)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Size of Serialized Data File – Binary data (GB)</t>
   </si>
 </sst>
 </file>
@@ -68,6 +74,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -89,9 +96,10 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -102,6 +110,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCCCC"/>
         <bgColor rgb="FFCCCCFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -146,7 +160,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -160,6 +174,26 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -240,18 +274,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+      <selection pane="topLeft" activeCell="F28" activeCellId="0" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.4183673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.9234693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.8571428571429"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3214285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.8775510204082"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -460,10 +494,198 @@
         <v>4.967326162</v>
       </c>
     </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="6" t="n">
+        <v>152.525</v>
+      </c>
+      <c r="C19" s="6" t="n">
+        <v>540.335</v>
+      </c>
+      <c r="D19" s="6" t="n">
+        <v>74.6807</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="6" t="n">
+        <v>106.683</v>
+      </c>
+      <c r="C20" s="6" t="n">
+        <v>333.878</v>
+      </c>
+      <c r="D20" s="6" t="n">
+        <v>66.2949</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="6" t="n">
+        <v>59.7214</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="6" t="n">
+        <v>88.2539</v>
+      </c>
+      <c r="C22" s="6" t="n">
+        <v>289.556</v>
+      </c>
+      <c r="D22" s="6" t="n">
+        <v>79.3396</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="6" t="n">
+        <v>70.4635</v>
+      </c>
+      <c r="C23" s="6" t="n">
+        <v>187.176</v>
+      </c>
+      <c r="D23" s="6" t="n">
+        <v>58.7767</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="7" t="n">
+        <v>3.0423783156</v>
+      </c>
+      <c r="C27" s="7" t="n">
+        <v>9.982511392</v>
+      </c>
+      <c r="D27" s="7" t="n">
+        <v>1.932985173</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="7" t="n">
+        <v>2.161175274</v>
+      </c>
+      <c r="C28" s="7" t="n">
+        <v>6.587253146</v>
+      </c>
+      <c r="D28" s="7" t="n">
+        <v>1.791065978</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="7" t="n">
+        <v>1.662723961</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" s="7" t="n">
+        <v>2.049469209</v>
+      </c>
+      <c r="C30" s="7" t="n">
+        <v>5.3057694</v>
+      </c>
+      <c r="D30" s="7" t="n">
+        <v>2.575099527</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" s="7" t="n">
+        <v>1.484849567</v>
+      </c>
+      <c r="C31" s="7" t="n">
+        <v>3.522409574</v>
+      </c>
+      <c r="D31" s="7" t="n">
+        <v>1.798093953</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A25:D25"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>